<commit_message>
Sprint 5 Complete, added Test Review Documents as well
</commit_message>
<xml_diff>
--- a/11. Sprint Planning and Review/Sprint 5 (10 - 17 May 2020)/Sprint 5 Burndown Chart.xlsx
+++ b/11. Sprint Planning and Review/Sprint 5 (10 - 17 May 2020)/Sprint 5 Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/804ce03f3a9950f7/Documents/MSSA/01. San Diego (Cloud Application Developer)/03. CAD Project/11. Sprint Planning and Review/Sprint 5 (10 - 17 May 2020)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{0778C0BB-4BF4-4A16-8B4F-3D03C53B2311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81127A54-84C0-4B70-B59E-AEE6DBA56237}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{0778C0BB-4BF4-4A16-8B4F-3D03C53B2311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3B16F77-003C-4969-9608-30DD5E0E1559}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE03FF15-3D1E-4EC4-9438-EDE4E738FADC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Sprint 4: 03 - 10 May 2020</t>
+  </si>
+  <si>
+    <t>Sprint 4: 10 - 17 May 2020</t>
   </si>
 </sst>
 </file>
@@ -168,10 +171,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -235,7 +238,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>(as of  09MAY2020)</a:t>
+              <a:t>(as of  16MAY2020)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -372,28 +375,28 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>43954</c:v>
+                  <c:v>43961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955</c:v>
+                  <c:v>43962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43956</c:v>
+                  <c:v>43963</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43957</c:v>
+                  <c:v>43964</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43958</c:v>
+                  <c:v>43965</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43959</c:v>
+                  <c:v>43966</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43960</c:v>
+                  <c:v>43967</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43961</c:v>
+                  <c:v>43968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,28 +408,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,28 +538,28 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>43954</c:v>
+                  <c:v>43961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955</c:v>
+                  <c:v>43962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43956</c:v>
+                  <c:v>43963</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43957</c:v>
+                  <c:v>43964</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43958</c:v>
+                  <c:v>43965</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43959</c:v>
+                  <c:v>43966</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43960</c:v>
+                  <c:v>43967</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43961</c:v>
+                  <c:v>43968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,28 +571,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-5</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5938,7 +5941,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5954,7 +5957,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -5968,11 +5971,11 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="12">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="D2" s="11">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5996,7 +5999,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="B4" s="8">
         <v>0</v>
@@ -6006,19 +6009,19 @@
       </c>
       <c r="D4" s="8">
         <f>$D$2+SUM(C4)-SUM(B4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>D2</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>43955</v>
+        <v>43962</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -6028,19 +6031,19 @@
       </c>
       <c r="D5" s="8">
         <f>$D$2+SUM(C4:C5)-SUM(B4:B5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8">
         <f>$D$2-SUM(E4:E5)</f>
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>43956</v>
+        <v>43963</v>
       </c>
       <c r="B6" s="8">
         <v>0</v>
@@ -6050,19 +6053,19 @@
       </c>
       <c r="D6" s="8">
         <f>$D$2+SUM(C4:C6)-SUM(B4:B6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="8">
         <f>$D$2-SUM(E4:E6)</f>
-        <v>-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>43957</v>
+        <v>43964</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -6072,85 +6075,84 @@
       </c>
       <c r="D7" s="8">
         <f>$D$2+SUM(C4:C7)-SUM(B4:B7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8">
         <f>$D$2-SUM(E4:E7)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>43958</v>
+        <v>43965</v>
       </c>
       <c r="B8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
       </c>
       <c r="D8" s="8">
         <f>$D$2+SUM(C4:C8)-SUM(B4:B8)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="8">
         <f>$D$2-SUM(E4:E8)</f>
-        <v>-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>43959</v>
+        <v>43966</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
       </c>
       <c r="D9" s="8">
         <f>$D$2+SUM(C4:C9)-SUM(B4:B9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" s="8">
         <v>1</v>
       </c>
       <c r="F9" s="8">
         <f>$D$2-SUM(E4:E9)</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>43960</v>
+        <v>43967</v>
       </c>
       <c r="B10" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
       </c>
       <c r="D10" s="8">
         <f>$D$2+SUM(C4:C10)-SUM(B4:B10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="8">
         <v>1</v>
       </c>
       <c r="F10" s="8">
-        <f>$D$2-SUM(E4:E10)</f>
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>43961</v>
+        <v>43968</v>
       </c>
       <c r="B11" s="8">
         <v>0</v>
@@ -6160,15 +6162,14 @@
       </c>
       <c r="D11" s="8">
         <f>$D$2+SUM(C4:C11)-SUM(B4:B11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" ref="E11" si="0">_xlfn.CEILING.MATH(($D$2/7),1)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
         <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <f>$D$2-SUM(E4:E11)</f>
-        <v>-6</v>
       </c>
     </row>
   </sheetData>
@@ -6218,11 +6219,11 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>8</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6468,11 +6469,11 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>6</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6719,11 +6720,11 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="11">
+      <c r="D2" s="12">
         <v>5</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>